<commit_message>
update: check possible algorithm on data
</commit_message>
<xml_diff>
--- a/inst/extdata/help_algorithms.xlsx
+++ b/inst/extdata/help_algorithms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\OE\FG32\Mitarbeitende\VietorA\Projekte\U4S\Repositories\signal-detection-tool\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alena\Repositories\Sonstiges\signal-detection-tool\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF3EE64-1D34-4365-B102-CE1AEC09BE2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5165FA-B48E-4E07-9B80-A108A487C692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{A51CCECE-9157-496F-8864-AE08B7B68C33}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A51CCECE-9157-496F-8864-AE08B7B68C33}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>2 years</t>
   </si>
   <si>
-    <t>1 year</t>
-  </si>
-  <si>
     <t>1.5 years</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Signal detection algorithm</t>
+  </si>
+  <si>
+    <t>26 weeks</t>
   </si>
 </sst>
 </file>
@@ -155,9 +155,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -195,7 +195,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -301,7 +301,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -443,7 +443,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -454,18 +454,18 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -474,10 +474,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -488,10 +488,10 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -502,10 +502,10 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -516,10 +516,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -530,10 +530,10 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -547,7 +547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -561,7 +561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -575,7 +575,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -589,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>

</xml_diff>